<commit_message>
Add sub annual COM_FR for solar and space heat, and NCAP_AF for retrofit in RSD
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_SubAnnual_Data.xlsx
+++ b/SuppXLS/Scen_SYS_SubAnnual_Data.xlsx
@@ -7,14 +7,17 @@
   </bookViews>
   <sheets>
     <sheet name="TimeSlices" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PWR_AF" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TRA_DEM" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="RSDSOL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RSD_SH" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="RSD_RTFT" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PWR_AF" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TRA_DEM" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">~TFM_INS</t>
   </si>
@@ -115,15 +118,30 @@
     <t xml:space="preserve">YRFR</t>
   </si>
   <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cset_CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM_FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSDSOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSDSH*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pset_PN</t>
   </si>
   <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
     <t xml:space="preserve">NCAP_AF</t>
   </si>
   <si>
+    <t xml:space="preserve">R-RTFT*</t>
+  </si>
+  <si>
     <t xml:space="preserve">P-RNW-WIN-ON*</t>
   </si>
   <si>
@@ -146,9 +164,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cset_CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM_FR</t>
   </si>
   <si>
     <t xml:space="preserve">DEM</t>
@@ -241,13 +256,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="pwr_af" displayName="pwr_af" ref="B2:G8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:G8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="rsdsol" displayName="rsdsol" ref="B2:G3" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B2:G3"/>
   <tableColumns count="6">
     <tableColumn id="1" name="TimeSlice"/>
     <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="Pset_PN"/>
-    <tableColumn id="4" name="Year"/>
+    <tableColumn id="3" name="Year"/>
+    <tableColumn id="4" name="Cset_CN"/>
     <tableColumn id="5" name="IE"/>
     <tableColumn id="6" name="National"/>
   </tableColumns>
@@ -256,7 +271,52 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="tra_dem" displayName="tra_dem" ref="B2:AG3" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="rsd_sh" displayName="rsd_sh" ref="B2:G3" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B2:G3"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="TimeSlice"/>
+    <tableColumn id="2" name="Attribute"/>
+    <tableColumn id="3" name="Year"/>
+    <tableColumn id="4" name="Cset_CN"/>
+    <tableColumn id="5" name="IE"/>
+    <tableColumn id="6" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rsd_rtft" displayName="rsd_rtft" ref="B2:G3" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B2:G3"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="TimeSlice"/>
+    <tableColumn id="2" name="Attribute"/>
+    <tableColumn id="3" name="Year"/>
+    <tableColumn id="4" name="Pset_PN"/>
+    <tableColumn id="5" name="IE"/>
+    <tableColumn id="6" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="pwr_af" displayName="pwr_af" ref="B2:G8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B2:G8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="TimeSlice"/>
+    <tableColumn id="2" name="Attribute"/>
+    <tableColumn id="3" name="Year"/>
+    <tableColumn id="4" name="Pset_PN"/>
+    <tableColumn id="5" name="IE"/>
+    <tableColumn id="6" name="National"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="tra_dem" displayName="tra_dem" ref="B2:AG3" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="B2:AG3"/>
   <tableColumns count="32">
     <tableColumn id="1" name="TimeSlice"/>
@@ -819,117 +879,17 @@
       <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="n">
-        <v>2018</v>
-      </c>
       <c r="F3" t="n">
-        <v>0.2906</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2906</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.28925</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.28925</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.10802</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.10802</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.10802</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.10802</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.4122</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.4122</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2018</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -962,94 +922,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -1057,96 +939,18 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D3" t="n">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1157,4 +961,446 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.2906</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.2906</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.28925</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.28925</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.10802</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.10802</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.10802</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.10802</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.4122</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.4122</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId8"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove AF for SRV PV from SubAnnual
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_SubAnnual_Data.xlsx
+++ b/SuppXLS/Scen_SYS_SubAnnual_Data.xlsx
@@ -1,183 +1,187 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886FB9DB-2B2D-439F-98F2-68DD3B84BA11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TimeSlices" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="RSDSOL" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RSD_SH" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="RSD_RTFT" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="PWR_AF" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TRA_DEM" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TimeSlices" sheetId="1" r:id="rId1"/>
+    <sheet name="RSDSOL" sheetId="2" r:id="rId2"/>
+    <sheet name="RSD_SH" sheetId="3" r:id="rId3"/>
+    <sheet name="RSD_RTFT" sheetId="4" r:id="rId4"/>
+    <sheet name="PWR_AF" sheetId="5" r:id="rId5"/>
+    <sheet name="TRA_DEM" sheetId="6" r:id="rId6"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
-  <si>
-    <t xml:space="preserve">~TFM_INS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimeSlice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-CW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-KE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-KK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-LS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-LD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-LH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-MH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-OY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-WH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-WX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-WW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-CE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-KY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-LK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-TA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-WD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-LM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-MO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-RN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-SO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-DL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE-MN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YRFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cset_CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM_FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSDSOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSDSH*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pset_PN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NCAP_AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R-RTFT*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-RNW-WIN-ON*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-RNW-WIN-OF*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-RNW-SOL-*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPVELC*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-RNW*WAV*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-RNW*TID*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cset_set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cset_CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport Demand*</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>IE-CW</t>
+  </si>
+  <si>
+    <t>IE-D</t>
+  </si>
+  <si>
+    <t>IE-KE</t>
+  </si>
+  <si>
+    <t>IE-KK</t>
+  </si>
+  <si>
+    <t>IE-LS</t>
+  </si>
+  <si>
+    <t>IE-LD</t>
+  </si>
+  <si>
+    <t>IE-LH</t>
+  </si>
+  <si>
+    <t>IE-MH</t>
+  </si>
+  <si>
+    <t>IE-OY</t>
+  </si>
+  <si>
+    <t>IE-WH</t>
+  </si>
+  <si>
+    <t>IE-WX</t>
+  </si>
+  <si>
+    <t>IE-WW</t>
+  </si>
+  <si>
+    <t>IE-CE</t>
+  </si>
+  <si>
+    <t>IE-CO</t>
+  </si>
+  <si>
+    <t>IE-KY</t>
+  </si>
+  <si>
+    <t>IE-LK</t>
+  </si>
+  <si>
+    <t>IE-TA</t>
+  </si>
+  <si>
+    <t>IE-WD</t>
+  </si>
+  <si>
+    <t>IE-G</t>
+  </si>
+  <si>
+    <t>IE-LM</t>
+  </si>
+  <si>
+    <t>IE-MO</t>
+  </si>
+  <si>
+    <t>IE-RN</t>
+  </si>
+  <si>
+    <t>IE-SO</t>
+  </si>
+  <si>
+    <t>IE-CN</t>
+  </si>
+  <si>
+    <t>IE-DL</t>
+  </si>
+  <si>
+    <t>IE-MN</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>YRFR</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Cset_CN</t>
+  </si>
+  <si>
+    <t>COM_FR</t>
+  </si>
+  <si>
+    <t>RSDSOL</t>
+  </si>
+  <si>
+    <t>RSDSH*</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>NCAP_AF</t>
+  </si>
+  <si>
+    <t>R-RTFT*</t>
+  </si>
+  <si>
+    <t>P-RNW-WIN-ON*</t>
+  </si>
+  <si>
+    <t>P-RNW-WIN-OF*</t>
+  </si>
+  <si>
+    <t>P-RNW-SOL-*</t>
+  </si>
+  <si>
+    <t>P-RNW*WAV*</t>
+  </si>
+  <si>
+    <t>P-RNW*TID*</t>
+  </si>
+  <si>
+    <t>Cset_set</t>
+  </si>
+  <si>
+    <t>Cset_CD</t>
+  </si>
+  <si>
+    <t>DEM</t>
+  </si>
+  <si>
+    <t>Transport Demand*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,144 +217,153 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="timeslices" displayName="timeslices" ref="B2:AE3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:AE3"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="timeslices" displayName="timeslices" ref="B2:AE3" totalsRowShown="0">
+  <autoFilter ref="B2:AE3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="30">
-    <tableColumn id="1" name="TimeSlice"/>
-    <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="IE"/>
-    <tableColumn id="4" name="National"/>
-    <tableColumn id="5" name="IE-CW"/>
-    <tableColumn id="6" name="IE-D"/>
-    <tableColumn id="7" name="IE-KE"/>
-    <tableColumn id="8" name="IE-KK"/>
-    <tableColumn id="9" name="IE-LS"/>
-    <tableColumn id="10" name="IE-LD"/>
-    <tableColumn id="11" name="IE-LH"/>
-    <tableColumn id="12" name="IE-MH"/>
-    <tableColumn id="13" name="IE-OY"/>
-    <tableColumn id="14" name="IE-WH"/>
-    <tableColumn id="15" name="IE-WX"/>
-    <tableColumn id="16" name="IE-WW"/>
-    <tableColumn id="17" name="IE-CE"/>
-    <tableColumn id="18" name="IE-CO"/>
-    <tableColumn id="19" name="IE-KY"/>
-    <tableColumn id="20" name="IE-LK"/>
-    <tableColumn id="21" name="IE-TA"/>
-    <tableColumn id="22" name="IE-WD"/>
-    <tableColumn id="23" name="IE-G"/>
-    <tableColumn id="24" name="IE-LM"/>
-    <tableColumn id="25" name="IE-MO"/>
-    <tableColumn id="26" name="IE-RN"/>
-    <tableColumn id="27" name="IE-SO"/>
-    <tableColumn id="28" name="IE-CN"/>
-    <tableColumn id="29" name="IE-DL"/>
-    <tableColumn id="30" name="IE-MN"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="National"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IE-CW"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="IE-D"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IE-KE"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="IE-KK"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IE-LS"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IE-LD"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="IE-LH"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="IE-MH"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="IE-OY"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IE-WH"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IE-WX"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IE-WW"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="IE-CE"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="IE-CO"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="IE-KY"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="IE-LK"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="IE-TA"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IE-WD"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IE-G"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IE-LM"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="IE-MO"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="IE-RN"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="IE-SO"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IE-CN"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IE-DL"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="IE-MN"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="rsdsol" displayName="rsdsol" ref="B2:G3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:G3"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:G3" totalsRowShown="0">
+  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="TimeSlice"/>
-    <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="Year"/>
-    <tableColumn id="4" name="Cset_CN"/>
-    <tableColumn id="5" name="IE"/>
-    <tableColumn id="6" name="National"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Cset_CN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="National"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="rsd_sh" displayName="rsd_sh" ref="B2:G3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:G3"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:G3" totalsRowShown="0">
+  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="TimeSlice"/>
-    <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="Year"/>
-    <tableColumn id="4" name="Cset_CN"/>
-    <tableColumn id="5" name="IE"/>
-    <tableColumn id="6" name="National"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Cset_CN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="National"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="rsd_rtft" displayName="rsd_rtft" ref="B2:G3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:G3"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:G3" totalsRowShown="0">
+  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="TimeSlice"/>
-    <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="Year"/>
-    <tableColumn id="4" name="Pset_PN"/>
-    <tableColumn id="5" name="IE"/>
-    <tableColumn id="6" name="National"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="National"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="pwr_af" displayName="pwr_af" ref="B2:G8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:G8"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="pwr_af" displayName="pwr_af" ref="B2:G7" totalsRowShown="0">
+  <autoFilter ref="B2:G7" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="TimeSlice"/>
-    <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="Year"/>
-    <tableColumn id="4" name="Pset_PN"/>
-    <tableColumn id="5" name="IE"/>
-    <tableColumn id="6" name="National"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Pset_PN"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="IE"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="National"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="tra_dem" displayName="tra_dem" ref="B2:AG3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B2:AG3"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tra_dem" displayName="tra_dem" ref="B2:AG3" totalsRowShown="0">
+  <autoFilter ref="B2:AG3" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="32">
-    <tableColumn id="1" name="TimeSlice"/>
-    <tableColumn id="2" name="Attribute"/>
-    <tableColumn id="3" name="Year"/>
-    <tableColumn id="4" name="Cset_set"/>
-    <tableColumn id="5" name="Cset_CD"/>
-    <tableColumn id="6" name="IE"/>
-    <tableColumn id="7" name="IE-CW"/>
-    <tableColumn id="8" name="IE-KK"/>
-    <tableColumn id="9" name="IE-LS"/>
-    <tableColumn id="10" name="IE-LD"/>
-    <tableColumn id="11" name="IE-LH"/>
-    <tableColumn id="12" name="IE-OY"/>
-    <tableColumn id="13" name="IE-WH"/>
-    <tableColumn id="14" name="IE-WX"/>
-    <tableColumn id="15" name="IE-CE"/>
-    <tableColumn id="16" name="IE-KY"/>
-    <tableColumn id="17" name="IE-TA"/>
-    <tableColumn id="18" name="IE-LM"/>
-    <tableColumn id="19" name="IE-MO"/>
-    <tableColumn id="20" name="IE-RN"/>
-    <tableColumn id="21" name="IE-SO"/>
-    <tableColumn id="22" name="IE-CN"/>
-    <tableColumn id="23" name="IE-DL"/>
-    <tableColumn id="24" name="IE-MN"/>
-    <tableColumn id="25" name="IE-D"/>
-    <tableColumn id="26" name="IE-KE"/>
-    <tableColumn id="27" name="IE-MH"/>
-    <tableColumn id="28" name="IE-WW"/>
-    <tableColumn id="29" name="IE-CO"/>
-    <tableColumn id="30" name="IE-LK"/>
-    <tableColumn id="31" name="IE-WD"/>
-    <tableColumn id="32" name="IE-G"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="TimeSlice"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Cset_set"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Cset_CD"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="IE"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="IE-CW"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="IE-KK"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="IE-LS"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="IE-LD"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="IE-LH"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="IE-OY"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="IE-WH"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="IE-WX"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="IE-CE"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="IE-KY"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="IE-TA"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="IE-LM"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0500-000013000000}" name="IE-MO"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0500-000014000000}" name="IE-RN"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0500-000015000000}" name="IE-SO"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0500-000016000000}" name="IE-CN"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0500-000017000000}" name="IE-DL"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0500-000018000000}" name="IE-MN"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0500-000019000000}" name="IE-D"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0500-00001A000000}" name="IE-KE"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0500-00001B000000}" name="IE-MH"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0500-00001C000000}" name="IE-WW"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0500-00001D000000}" name="IE-CO"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0500-00001E000000}" name="IE-LK"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0500-00001F000000}" name="IE-WD"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0500-000020000000}" name="IE-G"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -634,19 +647,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -738,121 +751,121 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE3" t="n">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -872,49 +885,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -934,49 +947,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -996,49 +1009,51 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1058,149 +1073,129 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.2906</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.2906</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="F3">
+        <v>0.29060000000000002</v>
+      </c>
+      <c r="G3">
+        <v>0.29060000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>2018</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.28925</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.28925</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="F4">
+        <v>0.28925000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.28925000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>2018</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>0.10802</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>0.10802</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>2018</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.10802</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.10802</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="F6">
+        <v>0.41220000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.41220000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>2018</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="n">
-        <v>0.4122</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.4122</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2018</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="F7">
         <v>0.3</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G7">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1211,10 +1206,10 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1298,109 +1293,109 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2018</v>
       </c>
       <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG3" t="n">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>